<commit_message>
apply delete test case
</commit_message>
<xml_diff>
--- a/MavenGit/src/main/java/File/TestCase.xlsx
+++ b/MavenGit/src/main/java/File/TestCase.xlsx
@@ -407,7 +407,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -444,10 +444,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -461,10 +461,10 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -478,10 +478,10 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -495,10 +495,10 @@
         <v>12</v>
       </c>
       <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
         <v>2</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>

</xml_diff>